<commit_message>
Updated TS correction and coef for archaeology
</commit_message>
<xml_diff>
--- a/default_sum_koef.xlsx
+++ b/default_sum_koef.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0E5E97-8A78-7846-A824-BBC48EE7E75F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77367460-CE25-4F4E-B023-22A97E3E7CCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total sum" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Ca44</t>
   </si>
@@ -37,15 +37,9 @@
     <t>Ti47</t>
   </si>
   <si>
-    <t>Ta181</t>
-  </si>
-  <si>
     <t>Mn55</t>
   </si>
   <si>
-    <t>Nb93</t>
-  </si>
-  <si>
     <t>Si28</t>
   </si>
   <si>
@@ -58,19 +52,64 @@
     <t>Pb208</t>
   </si>
   <si>
+    <t>Cu63</t>
+  </si>
+  <si>
     <t>Fe56</t>
   </si>
   <si>
     <t>Sn118</t>
   </si>
   <si>
+    <t>74.186</t>
+  </si>
+  <si>
+    <t>60.304</t>
+  </si>
+  <si>
+    <t>52.925</t>
+  </si>
+  <si>
+    <t>46.75</t>
+  </si>
+  <si>
+    <t>43.64</t>
+  </si>
+  <si>
+    <t>83.01</t>
+  </si>
+  <si>
+    <t>71.469</t>
+  </si>
+  <si>
+    <t>59.934</t>
+  </si>
+  <si>
+    <t>77.44</t>
+  </si>
+  <si>
+    <t>69.943</t>
+  </si>
+  <si>
+    <t>78.65</t>
+  </si>
+  <si>
+    <t>79.88</t>
+  </si>
+  <si>
+    <t>78.77</t>
+  </si>
+  <si>
+    <t>83.53</t>
+  </si>
+  <si>
+    <t>92.83</t>
+  </si>
+  <si>
     <t>P31</t>
   </si>
   <si>
     <t>Co59</t>
-  </si>
-  <si>
-    <t>Cu65</t>
   </si>
 </sst>
 </file>
@@ -106,8 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,151 +433,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BED263DA-3ED2-499A-8427-FAFD0CB42F7F}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>74.186000000000007</v>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>60.304000000000002</v>
+      <c r="B2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>52.924999999999997</v>
+      <c r="B3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <v>46.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>43.64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>83.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>71.468999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>59.933999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>77.44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>69.942999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>78.650000000000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>79.88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>69.903999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>78.77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>83.53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>81.897999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>92.83</v>
+      <c r="B15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>